<commit_message>
Se suben los documentos actualizados
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 1.xlsx
+++ b/Fase 1/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 1.xlsx
@@ -38,7 +38,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="p6NiSgShZaUt6420Z7IRIvcnHQOMj+l6kYPvHduUXJs="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="YVyJ16Jjmt1Y1U/C1syV4muIOY7FHIOdRItHrLwYpAQ="/>
     </ext>
   </extLst>
 </workbook>
@@ -3575,10 +3575,6 @@
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="C39:K40"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="J53:K53"/>
     <mergeCell ref="D41:K41"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -3586,6 +3582,10 @@
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="C50:K51"/>
     <mergeCell ref="D52:K52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="J53:K53"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E6">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>